<commit_message>
Product Mix Problem Completed
</commit_message>
<xml_diff>
--- a/ProductMixProblem/Product_Mix_Problem.xlsx
+++ b/ProductMixProblem/Product_Mix_Problem.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HValuck\Desktop\Pyomo Optimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HValuck\Desktop\Pyomo Optimization\ProductMixProblem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{137A8C49-6055-4C2E-89AC-00B886788E57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88342F8-9FE5-4291-BFB6-3367F2081809}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39CCFCBB-AF22-4DC3-A24B-93845F8E8F3C}"/>
+    <workbookView xWindow="28692" yWindow="-2460" windowWidth="24216" windowHeight="13116" xr2:uid="{39CCFCBB-AF22-4DC3-A24B-93845F8E8F3C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Profit" sheetId="2" r:id="rId1"/>
-    <sheet name="Constraints" sheetId="3" r:id="rId2"/>
+    <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Profit</t>
   </si>
@@ -88,82 +87,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -180,10 +112,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -472,44 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33193D04-D495-4956-AEF2-82475292A2BA}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>2.25</v>
-      </c>
-      <c r="C2">
-        <v>2.6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800FA4E7-3E03-45F2-983B-6843E67BEE54}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -527,29 +425,41 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>4000</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C4" s="1">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D4" s="1">
         <v>5000</v>
       </c>
     </row>

</xml_diff>